<commit_message>
Mappingfil for næring tilpasset ny versjon
</commit_message>
<xml_diff>
--- a/docs/documentation/informasjonsmodell/Mapping-Xpath-Skjema-Orid.xlsx
+++ b/docs/documentation/informasjonsmodell/Mapping-Xpath-Skjema-Orid.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="842" uniqueCount="591">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="843" uniqueCount="592">
   <si>
     <t>Xpath</t>
   </si>
@@ -470,9 +470,6 @@
     <t>/naeringsopplysninger/virksomhet/selskapstype/selskapstype</t>
   </si>
   <si>
-    <t>/naeringsopplysninger/virksomhet/antallMaanederDrevetIAar/heltall</t>
-  </si>
-  <si>
     <t>Nytt felt: Angis hvis feltet erRealisasjonenUfrivilligOgGevinstenBetingetSkattefri/boolsk er true</t>
   </si>
   <si>
@@ -1797,6 +1794,12 @@
   </si>
   <si>
     <t>Nytt felt.  Benyttes til avkorting av skjermingsfrdrag ved drift i kun deler av året</t>
+  </si>
+  <si>
+    <t>/naeringsopplysninger/personinntektFraEnkeltpersonforetak/antallMaanederDrevetIAar/heltall</t>
+  </si>
+  <si>
+    <t>/naeringsopplysninger/spesifikasjonAvResultatregnskapOgBalanse/gevinstOgTapskonto/stammerGevinstOgTapskontoenFraGevinstFraRealisasjonAvAlminneligGaardsbrukEllerSkogbruk/boolsk</t>
   </si>
 </sst>
 </file>
@@ -2127,16 +2130,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J436"/>
+  <dimension ref="A1:J437"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="L426" sqref="L426"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="100.5546875" style="5" customWidth="1"/>
-    <col min="2" max="2" width="18.6640625" customWidth="1"/>
+    <col min="1" max="1" width="160.6640625" style="5" customWidth="1"/>
+    <col min="2" max="2" width="28.44140625" customWidth="1"/>
     <col min="3" max="3" width="16.33203125" customWidth="1"/>
     <col min="4" max="4" width="18" customWidth="1"/>
     <col min="5" max="5" width="6.88671875" customWidth="1"/>
@@ -2182,29 +2183,29 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="B4" t="s">
         <v>5</v>
       </c>
       <c r="D4" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="B5" t="s">
         <v>5</v>
       </c>
       <c r="D5" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B6" t="s">
         <v>5</v>
@@ -2226,15 +2227,15 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="H8" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" s="5" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="H9" t="s">
         <v>111</v>
@@ -2242,7 +2243,7 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" s="5" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="B10" t="s">
         <v>9</v>
@@ -2250,7 +2251,7 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" s="5" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="B11" t="s">
         <v>5</v>
@@ -2261,23 +2262,23 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" s="5" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="H12" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" s="5" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="H13" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" s="5" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="H14" t="s">
         <v>111</v>
@@ -2285,7 +2286,7 @@
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" s="5" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="B15" t="s">
         <v>7</v>
@@ -2293,7 +2294,7 @@
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" s="5" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="B16" t="s">
         <v>5</v>
@@ -2304,15 +2305,15 @@
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" s="5" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="H17" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" s="5" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B18" t="s">
         <v>5</v>
@@ -2334,15 +2335,15 @@
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20" s="5" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="H20" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21" s="5" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="H21" t="s">
         <v>111</v>
@@ -2350,7 +2351,7 @@
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22" s="5" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="B22" t="s">
         <v>10</v>
@@ -2358,7 +2359,7 @@
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A23" s="5" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="B23" t="s">
         <v>5</v>
@@ -2369,23 +2370,23 @@
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A24" s="5" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="H24" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A25" s="5" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="H25" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A26" s="5" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="H26" t="s">
         <v>111</v>
@@ -2393,7 +2394,7 @@
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A27" s="5" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="B27" t="s">
         <v>11</v>
@@ -2401,7 +2402,7 @@
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A28" s="5" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="B28" t="s">
         <v>5</v>
@@ -2412,23 +2413,23 @@
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A29" s="5" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="H29" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A30" s="5" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="H30" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A31" s="5" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="H31" t="s">
         <v>111</v>
@@ -2436,7 +2437,7 @@
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A32" s="5" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="B32" t="s">
         <v>12</v>
@@ -2444,7 +2445,7 @@
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A33" s="5" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="B33" t="s">
         <v>5</v>
@@ -2455,15 +2456,15 @@
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A34" s="5" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="H34" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A35" s="5" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B35" t="s">
         <v>5</v>
@@ -2485,7 +2486,7 @@
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A37" s="5" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B37" t="s">
         <v>5</v>
@@ -2507,7 +2508,7 @@
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A39" s="5" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B39" s="1"/>
       <c r="H39" t="s">
@@ -2524,7 +2525,7 @@
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A41" s="5" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="H41" t="s">
         <v>80</v>
@@ -2540,7 +2541,7 @@
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A43" s="5" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B43">
         <v>1167</v>
@@ -2562,7 +2563,7 @@
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A45" s="5" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B45" t="s">
         <v>5</v>
@@ -2593,15 +2594,15 @@
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A47" s="5" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="H47" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A48" s="5" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="H48" t="s">
         <v>111</v>
@@ -2609,7 +2610,7 @@
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A49" s="5" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="B49" t="s">
         <v>13</v>
@@ -2617,7 +2618,7 @@
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A50" s="5" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="B50" t="s">
         <v>5</v>
@@ -2628,23 +2629,23 @@
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A51" s="5" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="H51" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A52" s="5" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="H52" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A53" s="5" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="H53" t="s">
         <v>111</v>
@@ -2652,7 +2653,7 @@
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A54" s="5" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="B54" t="s">
         <v>14</v>
@@ -2660,7 +2661,7 @@
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A55" s="5" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="B55" t="s">
         <v>5</v>
@@ -2671,23 +2672,23 @@
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A56" s="5" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="H56" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A57" s="5" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="H57" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A58" s="5" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="H58" t="s">
         <v>111</v>
@@ -2695,7 +2696,7 @@
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A59" s="5" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="B59">
         <v>1167</v>
@@ -2709,7 +2710,7 @@
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A60" s="5" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="B60">
         <v>1167</v>
@@ -2723,23 +2724,23 @@
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A61" s="5" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="H61" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A62" s="5" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="H62" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A63" s="5" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="H63" t="s">
         <v>111</v>
@@ -2747,29 +2748,29 @@
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A64" s="5" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="B64">
         <v>1167</v>
       </c>
       <c r="C64" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A65" s="5" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="B65">
         <v>1167</v>
       </c>
       <c r="C65" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A66" s="5" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="B66" t="s">
         <v>15</v>
@@ -2777,23 +2778,23 @@
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A67" s="5" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="H67" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A68" s="5" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="H68" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A69" s="5" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="H69" t="s">
         <v>111</v>
@@ -2801,7 +2802,7 @@
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A70" s="5" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="B70" t="s">
         <v>105</v>
@@ -2809,7 +2810,7 @@
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A71" s="5" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="B71">
         <v>1167</v>
@@ -2820,15 +2821,15 @@
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A72" s="5" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="H72" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A73" s="5" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="H73" t="s">
         <v>81</v>
@@ -2844,7 +2845,7 @@
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A75" s="5" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="H75" t="s">
         <v>82</v>
@@ -2860,23 +2861,23 @@
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A77" s="5" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="H77" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A78" s="5" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="H78" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A79" s="5" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="H79" t="s">
         <v>111</v>
@@ -2884,7 +2885,7 @@
     </row>
     <row r="80" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A80" s="5" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="B80" t="s">
         <v>77</v>
@@ -2892,7 +2893,7 @@
     </row>
     <row r="81" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A81" s="5" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="B81" t="s">
         <v>5</v>
@@ -2903,7 +2904,7 @@
     </row>
     <row r="82" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A82" s="5" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="B82" t="s">
         <v>5</v>
@@ -2914,15 +2915,15 @@
     </row>
     <row r="83" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A83" s="5" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="H83" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
     </row>
     <row r="84" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A84" s="5" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="H84" t="s">
         <v>83</v>
@@ -2938,7 +2939,7 @@
     </row>
     <row r="86" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A86" s="5" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="H86" t="s">
         <v>84</v>
@@ -2954,23 +2955,23 @@
     </row>
     <row r="88" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A88" s="5" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="H88" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
     </row>
     <row r="89" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A89" s="5" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="H89" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
     </row>
     <row r="90" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A90" s="5" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="H90" t="s">
         <v>111</v>
@@ -2978,7 +2979,7 @@
     </row>
     <row r="91" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A91" s="5" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="B91" t="s">
         <v>78</v>
@@ -2986,7 +2987,7 @@
     </row>
     <row r="92" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A92" s="5" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="B92" t="s">
         <v>5</v>
@@ -2997,7 +2998,7 @@
     </row>
     <row r="93" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A93" s="5" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="B93" t="s">
         <v>5</v>
@@ -3008,15 +3009,15 @@
     </row>
     <row r="94" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A94" s="5" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="H94" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
     </row>
     <row r="95" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A95" s="5" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="H95" t="s">
         <v>85</v>
@@ -3024,7 +3025,7 @@
     </row>
     <row r="96" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A96" s="5" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="H96" t="s">
         <v>110</v>
@@ -3032,7 +3033,7 @@
     </row>
     <row r="97" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A97" s="5" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="H97" t="s">
         <v>86</v>
@@ -3040,7 +3041,7 @@
     </row>
     <row r="98" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A98" s="5" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="H98" t="s">
         <v>110</v>
@@ -3048,7 +3049,7 @@
     </row>
     <row r="99" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A99" s="5" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="H99" t="s">
         <v>87</v>
@@ -3056,7 +3057,7 @@
     </row>
     <row r="100" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A100" s="5" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="H100" t="s">
         <v>110</v>
@@ -3064,7 +3065,7 @@
     </row>
     <row r="101" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A101" s="5" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="H101" t="s">
         <v>88</v>
@@ -3072,7 +3073,7 @@
     </row>
     <row r="102" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A102" s="5" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="H102" t="s">
         <v>110</v>
@@ -3080,7 +3081,7 @@
     </row>
     <row r="103" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A103" s="5" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B103" t="s">
         <v>5</v>
@@ -3102,15 +3103,15 @@
     </row>
     <row r="105" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A105" s="5" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="H105" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
     </row>
     <row r="106" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A106" s="5" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="H106" t="s">
         <v>111</v>
@@ -3118,7 +3119,7 @@
     </row>
     <row r="107" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A107" s="5" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="B107" t="s">
         <v>64</v>
@@ -3126,7 +3127,7 @@
     </row>
     <row r="108" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A108" s="5" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="B108" t="s">
         <v>5</v>
@@ -3137,7 +3138,7 @@
     </row>
     <row r="109" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A109" s="5" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="B109" t="s">
         <v>5</v>
@@ -3148,31 +3149,31 @@
     </row>
     <row r="110" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A110" s="5" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="H110" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
     </row>
     <row r="111" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A111" s="5" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="H111" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
     </row>
     <row r="112" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A112" s="5" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="H112" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
     </row>
     <row r="113" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A113" s="5" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="H113" t="s">
         <v>111</v>
@@ -3180,7 +3181,7 @@
     </row>
     <row r="114" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A114" s="5" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="B114" t="s">
         <v>65</v>
@@ -3188,7 +3189,7 @@
     </row>
     <row r="115" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A115" s="5" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="B115" t="s">
         <v>5</v>
@@ -3199,7 +3200,7 @@
     </row>
     <row r="116" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A116" s="5" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="B116" t="s">
         <v>5</v>
@@ -3210,31 +3211,31 @@
     </row>
     <row r="117" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A117" s="5" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="H117" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
     </row>
     <row r="118" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A118" s="5" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="H118" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
     </row>
     <row r="119" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A119" s="5" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="H119" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
     </row>
     <row r="120" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A120" s="5" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="H120" t="s">
         <v>111</v>
@@ -3242,7 +3243,7 @@
     </row>
     <row r="121" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A121" s="5" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="B121" t="s">
         <v>8</v>
@@ -3250,7 +3251,7 @@
     </row>
     <row r="122" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A122" s="5" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="B122" t="s">
         <v>5</v>
@@ -3261,18 +3262,18 @@
     </row>
     <row r="123" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A123" s="5" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="H123" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
     </row>
     <row r="124" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A124" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="H124" t="s">
         <v>163</v>
-      </c>
-      <c r="H124" t="s">
-        <v>164</v>
       </c>
     </row>
     <row r="125" spans="1:8" x14ac:dyDescent="0.3">
@@ -3285,10 +3286,10 @@
     </row>
     <row r="126" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A126" s="5" t="s">
+        <v>164</v>
+      </c>
+      <c r="H126" t="s">
         <v>165</v>
-      </c>
-      <c r="H126" t="s">
-        <v>166</v>
       </c>
     </row>
     <row r="127" spans="1:8" x14ac:dyDescent="0.3">
@@ -3301,10 +3302,10 @@
     </row>
     <row r="128" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A128" s="5" t="s">
+        <v>166</v>
+      </c>
+      <c r="H128" t="s">
         <v>167</v>
-      </c>
-      <c r="H128" t="s">
-        <v>168</v>
       </c>
     </row>
     <row r="129" spans="1:8" x14ac:dyDescent="0.3">
@@ -3317,10 +3318,10 @@
     </row>
     <row r="130" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A130" s="5" t="s">
+        <v>168</v>
+      </c>
+      <c r="H130" t="s">
         <v>169</v>
-      </c>
-      <c r="H130" t="s">
-        <v>170</v>
       </c>
     </row>
     <row r="131" spans="1:8" x14ac:dyDescent="0.3">
@@ -3333,15 +3334,15 @@
     </row>
     <row r="132" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A132" s="5" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="H132" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
     </row>
     <row r="133" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A133" s="5" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="H133" t="s">
         <v>111</v>
@@ -3349,7 +3350,7 @@
     </row>
     <row r="134" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A134" s="5" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="H134" t="s">
         <v>66</v>
@@ -3357,7 +3358,7 @@
     </row>
     <row r="135" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A135" s="5" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B135" t="s">
         <v>67</v>
@@ -3368,7 +3369,7 @@
     </row>
     <row r="136" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A136" s="5" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B136" t="s">
         <v>67</v>
@@ -3385,7 +3386,7 @@
     </row>
     <row r="137" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A137" s="5" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="B137" t="s">
         <v>67</v>
@@ -3397,12 +3398,12 @@
         <v>67</v>
       </c>
       <c r="H137" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
     </row>
     <row r="138" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A138" s="5" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="H138" t="s">
         <v>89</v>
@@ -3410,7 +3411,7 @@
     </row>
     <row r="139" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A139" s="5" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B139" t="s">
         <v>23</v>
@@ -3424,7 +3425,7 @@
     </row>
     <row r="140" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A140" s="5" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B140">
         <v>1084</v>
@@ -3438,7 +3439,7 @@
     </row>
     <row r="141" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A141" s="5" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B141">
         <v>1084</v>
@@ -3452,7 +3453,7 @@
     </row>
     <row r="142" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A142" s="5" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B142" t="s">
         <v>23</v>
@@ -3466,12 +3467,12 @@
     </row>
     <row r="143" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A143" s="5" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
     </row>
     <row r="144" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A144" s="5" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="H144" t="s">
         <v>36</v>
@@ -3479,23 +3480,23 @@
     </row>
     <row r="145" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A145" s="5" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="H145" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="146" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A146" s="5" t="s">
+        <v>382</v>
+      </c>
+      <c r="H146" t="s">
         <v>383</v>
-      </c>
-      <c r="H146" t="s">
-        <v>384</v>
       </c>
     </row>
     <row r="147" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A147" s="5" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B147">
         <v>1084</v>
@@ -3509,7 +3510,7 @@
     </row>
     <row r="148" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A148" s="5" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="H148" t="s">
         <v>39</v>
@@ -3517,7 +3518,7 @@
     </row>
     <row r="149" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A149" s="5" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B149">
         <v>1084</v>
@@ -3531,7 +3532,7 @@
     </row>
     <row r="150" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A150" s="5" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="H150" t="s">
         <v>37</v>
@@ -3539,7 +3540,7 @@
     </row>
     <row r="151" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A151" s="5" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B151">
         <v>1084</v>
@@ -3553,7 +3554,7 @@
     </row>
     <row r="152" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A152" s="5" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="H152" t="s">
         <v>100</v>
@@ -3561,7 +3562,7 @@
     </row>
     <row r="153" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A153" s="5" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="H153" t="s">
         <v>110</v>
@@ -3569,15 +3570,15 @@
     </row>
     <row r="154" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A154" s="5" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="H154" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
     </row>
     <row r="155" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A155" s="5" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="H155" t="s">
         <v>111</v>
@@ -3585,7 +3586,7 @@
     </row>
     <row r="156" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A156" s="5" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B156" t="s">
         <v>5</v>
@@ -3599,7 +3600,7 @@
     </row>
     <row r="157" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A157" s="5" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B157">
         <v>1224</v>
@@ -3610,7 +3611,7 @@
     </row>
     <row r="158" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A158" s="5" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="H158" t="s">
         <v>90</v>
@@ -3618,7 +3619,7 @@
     </row>
     <row r="159" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A159" s="5" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B159">
         <v>1219</v>
@@ -3629,7 +3630,7 @@
     </row>
     <row r="160" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A160" s="5" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="B160">
         <v>1219</v>
@@ -3641,12 +3642,12 @@
         <v>98</v>
       </c>
       <c r="H160" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
     </row>
     <row r="161" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A161" s="5" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="B161">
         <v>1219</v>
@@ -3658,12 +3659,12 @@
         <v>98</v>
       </c>
       <c r="H161" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
     </row>
     <row r="162" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A162" s="5" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B162">
         <v>1219</v>
@@ -3674,7 +3675,7 @@
     </row>
     <row r="163" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A163" s="5" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B163">
         <v>1084</v>
@@ -3685,7 +3686,7 @@
     </row>
     <row r="164" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A164" s="5" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B164">
         <v>1084</v>
@@ -3699,7 +3700,7 @@
     </row>
     <row r="165" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A165" s="5" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B165">
         <v>1084</v>
@@ -3713,7 +3714,7 @@
     </row>
     <row r="166" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A166" s="5" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B166">
         <v>1084</v>
@@ -3721,7 +3722,7 @@
     </row>
     <row r="167" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A167" s="5" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B167">
         <v>1084</v>
@@ -3735,7 +3736,7 @@
     </row>
     <row r="168" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A168" s="5" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B168">
         <v>1084</v>
@@ -3749,7 +3750,7 @@
     </row>
     <row r="169" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A169" s="5" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B169">
         <v>1084</v>
@@ -3763,7 +3764,7 @@
     </row>
     <row r="170" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A170" s="5" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B170">
         <v>1084</v>
@@ -3777,7 +3778,7 @@
     </row>
     <row r="171" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A171" s="5" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B171">
         <v>1084</v>
@@ -3791,7 +3792,7 @@
     </row>
     <row r="172" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A172" s="5" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B172">
         <v>1084</v>
@@ -3805,7 +3806,7 @@
     </row>
     <row r="173" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A173" s="5" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B173">
         <v>1084</v>
@@ -3819,7 +3820,7 @@
     </row>
     <row r="174" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A174" s="5" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B174">
         <v>1084</v>
@@ -3833,7 +3834,7 @@
     </row>
     <row r="175" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A175" s="5" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B175">
         <v>1084</v>
@@ -3847,7 +3848,7 @@
     </row>
     <row r="176" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A176" s="5" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B176">
         <v>1084</v>
@@ -3861,7 +3862,7 @@
     </row>
     <row r="177" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A177" s="5" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B177">
         <v>1084</v>
@@ -3875,7 +3876,7 @@
     </row>
     <row r="178" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A178" s="5" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B178">
         <v>1084</v>
@@ -3883,7 +3884,7 @@
     </row>
     <row r="179" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A179" s="5" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B179">
         <v>1084</v>
@@ -3891,7 +3892,7 @@
     </row>
     <row r="180" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A180" s="5" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B180">
         <v>1084</v>
@@ -3905,7 +3906,7 @@
     </row>
     <row r="181" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A181" s="5" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="B181">
         <v>1084</v>
@@ -3917,12 +3918,12 @@
         <v>6915</v>
       </c>
       <c r="H181" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
     </row>
     <row r="182" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A182" s="5" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="B182">
         <v>1084</v>
@@ -3934,12 +3935,12 @@
         <v>6915</v>
       </c>
       <c r="H182" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
     </row>
     <row r="183" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A183" s="5" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B183" t="s">
         <v>23</v>
@@ -3953,7 +3954,7 @@
     </row>
     <row r="184" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A184" s="5" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="H184" t="s">
         <v>33</v>
@@ -3961,15 +3962,15 @@
     </row>
     <row r="185" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A185" s="5" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="H185" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
     </row>
     <row r="186" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A186" s="5" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="H186" t="s">
         <v>111</v>
@@ -3977,7 +3978,7 @@
     </row>
     <row r="187" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A187" s="5" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B187">
         <v>1084</v>
@@ -3991,7 +3992,7 @@
     </row>
     <row r="188" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A188" s="5" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B188">
         <v>1084</v>
@@ -4005,7 +4006,7 @@
     </row>
     <row r="189" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A189" s="5" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B189">
         <v>1084</v>
@@ -4019,15 +4020,15 @@
     </row>
     <row r="190" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A190" s="5" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="H190" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
     </row>
     <row r="191" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A191" s="5" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B191">
         <v>1084</v>
@@ -4041,7 +4042,7 @@
     </row>
     <row r="192" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A192" s="5" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B192">
         <v>1084</v>
@@ -4055,7 +4056,7 @@
     </row>
     <row r="193" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A193" s="5" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B193">
         <v>1084</v>
@@ -4069,7 +4070,7 @@
     </row>
     <row r="194" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A194" s="5" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B194">
         <v>1084</v>
@@ -4083,7 +4084,7 @@
     </row>
     <row r="195" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A195" s="5" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B195">
         <v>1084</v>
@@ -4097,7 +4098,7 @@
     </row>
     <row r="196" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A196" s="5" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="B196">
         <v>1084</v>
@@ -4111,7 +4112,7 @@
     </row>
     <row r="197" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A197" s="5" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="H197" t="s">
         <v>36</v>
@@ -4119,23 +4120,23 @@
     </row>
     <row r="198" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A198" s="5" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="H198" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="199" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A199" s="5" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="H199" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
     </row>
     <row r="200" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A200" s="5" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B200">
         <v>1084</v>
@@ -4149,7 +4150,7 @@
     </row>
     <row r="201" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A201" s="5" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="H201" t="s">
         <v>39</v>
@@ -4157,7 +4158,7 @@
     </row>
     <row r="202" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A202" s="5" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B202">
         <v>1084</v>
@@ -4171,7 +4172,7 @@
     </row>
     <row r="203" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A203" s="5" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="H203" t="s">
         <v>37</v>
@@ -4179,7 +4180,7 @@
     </row>
     <row r="204" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A204" s="5" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B204">
         <v>1084</v>
@@ -4193,7 +4194,7 @@
     </row>
     <row r="205" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A205" s="5" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B205">
         <v>1084</v>
@@ -4207,7 +4208,7 @@
     </row>
     <row r="206" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A206" s="5" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="H206" t="s">
         <v>110</v>
@@ -4215,15 +4216,15 @@
     </row>
     <row r="207" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A207" s="5" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="H207" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
     </row>
     <row r="208" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A208" s="5" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="H208" t="s">
         <v>111</v>
@@ -4231,7 +4232,7 @@
     </row>
     <row r="209" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A209" s="5" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B209" t="s">
         <v>5</v>
@@ -4245,7 +4246,7 @@
     </row>
     <row r="210" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A210" s="5" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B210">
         <v>1224</v>
@@ -4256,7 +4257,7 @@
     </row>
     <row r="211" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A211" s="5" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="H211" t="s">
         <v>90</v>
@@ -4264,7 +4265,7 @@
     </row>
     <row r="212" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A212" s="5" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B212">
         <v>1219</v>
@@ -4275,7 +4276,7 @@
     </row>
     <row r="213" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A213" s="5" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="B213">
         <v>1219</v>
@@ -4287,12 +4288,12 @@
         <v>98</v>
       </c>
       <c r="H213" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
     </row>
     <row r="214" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A214" s="5" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="B214">
         <v>1219</v>
@@ -4304,12 +4305,12 @@
         <v>98</v>
       </c>
       <c r="H214" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
     </row>
     <row r="215" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A215" s="5" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B215">
         <v>1219</v>
@@ -4320,7 +4321,7 @@
     </row>
     <row r="216" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A216" s="5" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B216">
         <v>1084</v>
@@ -4331,7 +4332,7 @@
     </row>
     <row r="217" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A217" s="5" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B217">
         <v>1084</v>
@@ -4345,7 +4346,7 @@
     </row>
     <row r="218" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A218" s="5" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="B218">
         <v>1084</v>
@@ -4359,7 +4360,7 @@
     </row>
     <row r="219" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A219" s="5" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="B219">
         <v>1084</v>
@@ -4367,7 +4368,7 @@
     </row>
     <row r="220" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A220" s="5" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B220">
         <v>1084</v>
@@ -4381,7 +4382,7 @@
     </row>
     <row r="221" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A221" s="5" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B221">
         <v>1084</v>
@@ -4395,7 +4396,7 @@
     </row>
     <row r="222" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A222" s="5" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B222">
         <v>1084</v>
@@ -4409,7 +4410,7 @@
     </row>
     <row r="223" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A223" s="5" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B223">
         <v>1084</v>
@@ -4423,7 +4424,7 @@
     </row>
     <row r="224" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A224" s="5" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B224">
         <v>1084</v>
@@ -4437,7 +4438,7 @@
     </row>
     <row r="225" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A225" s="5" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="B225">
         <v>1084</v>
@@ -4451,7 +4452,7 @@
     </row>
     <row r="226" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A226" s="5" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="B226">
         <v>1084</v>
@@ -4465,7 +4466,7 @@
     </row>
     <row r="227" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A227" s="5" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B227">
         <v>1084</v>
@@ -4479,7 +4480,7 @@
     </row>
     <row r="228" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A228" s="5" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="B228">
         <v>1084</v>
@@ -4493,7 +4494,7 @@
     </row>
     <row r="229" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A229" s="5" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B229">
         <v>1084</v>
@@ -4507,7 +4508,7 @@
     </row>
     <row r="230" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A230" s="5" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="B230">
         <v>1084</v>
@@ -4521,7 +4522,7 @@
     </row>
     <row r="231" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A231" s="5" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="B231">
         <v>1084</v>
@@ -4529,7 +4530,7 @@
     </row>
     <row r="232" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A232" s="5" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B232">
         <v>1084</v>
@@ -4537,7 +4538,7 @@
     </row>
     <row r="233" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A233" s="5" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="B233">
         <v>1084</v>
@@ -4551,7 +4552,7 @@
     </row>
     <row r="234" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A234" s="5" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="B234">
         <v>1084</v>
@@ -4563,12 +4564,12 @@
         <v>6915</v>
       </c>
       <c r="H234" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
     </row>
     <row r="235" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A235" s="5" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="B235">
         <v>1084</v>
@@ -4580,12 +4581,12 @@
         <v>6915</v>
       </c>
       <c r="H235" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
     </row>
     <row r="236" spans="1:8" ht="13.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A236" s="5" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="B236">
         <v>1084</v>
@@ -4599,7 +4600,7 @@
     </row>
     <row r="237" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A237" s="5" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="H237" t="s">
         <v>110</v>
@@ -4607,7 +4608,7 @@
     </row>
     <row r="238" spans="1:8" ht="13.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A238" s="5" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="B238">
         <v>1084</v>
@@ -4621,7 +4622,7 @@
     </row>
     <row r="239" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A239" s="5" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="B239">
         <v>1084</v>
@@ -4635,7 +4636,7 @@
     </row>
     <row r="240" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A240" s="5" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B240">
         <v>1084</v>
@@ -4649,7 +4650,7 @@
     </row>
     <row r="241" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A241" s="5" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B241">
         <v>1084</v>
@@ -4663,7 +4664,7 @@
     </row>
     <row r="242" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A242" s="5" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B242">
         <v>1084</v>
@@ -4677,7 +4678,7 @@
     </row>
     <row r="243" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A243" s="5" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="B243">
         <v>1084</v>
@@ -4688,7 +4689,7 @@
     </row>
     <row r="244" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A244" s="5" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="B244">
         <v>1084</v>
@@ -4697,12 +4698,12 @@
         <v>112</v>
       </c>
       <c r="H244" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
     </row>
     <row r="245" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A245" s="5" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="B245">
         <v>1084</v>
@@ -4711,12 +4712,12 @@
         <v>112</v>
       </c>
       <c r="H245" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
     <row r="246" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A246" s="5" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="B246">
         <v>1084</v>
@@ -4730,7 +4731,7 @@
     </row>
     <row r="247" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A247" s="5" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="B247">
         <v>1084</v>
@@ -4744,7 +4745,7 @@
     </row>
     <row r="248" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A248" s="5" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="B248">
         <v>1084</v>
@@ -4758,15 +4759,15 @@
     </row>
     <row r="249" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A249" s="5" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="H249" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
     </row>
     <row r="250" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A250" s="5" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="H250" t="s">
         <v>111</v>
@@ -4774,7 +4775,7 @@
     </row>
     <row r="251" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A251" s="5" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="B251">
         <v>1084</v>
@@ -4788,7 +4789,7 @@
     </row>
     <row r="252" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A252" s="5" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B252">
         <v>1084</v>
@@ -4802,7 +4803,7 @@
     </row>
     <row r="253" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A253" s="5" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B253">
         <v>1084</v>
@@ -4816,15 +4817,15 @@
     </row>
     <row r="254" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A254" s="5" t="s">
+        <v>400</v>
+      </c>
+      <c r="H254" t="s">
         <v>401</v>
-      </c>
-      <c r="H254" t="s">
-        <v>402</v>
       </c>
     </row>
     <row r="255" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A255" s="5" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="B255">
         <v>1084</v>
@@ -4838,7 +4839,7 @@
     </row>
     <row r="256" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A256" s="5" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="B256">
         <v>1084</v>
@@ -4852,7 +4853,7 @@
     </row>
     <row r="257" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A257" s="5" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="B257">
         <v>1084</v>
@@ -4866,7 +4867,7 @@
     </row>
     <row r="258" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A258" s="5" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B258">
         <v>1084</v>
@@ -4880,7 +4881,7 @@
     </row>
     <row r="259" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A259" s="5" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="H259" t="s">
         <v>33</v>
@@ -4888,7 +4889,7 @@
     </row>
     <row r="260" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A260" s="5" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="H260" t="s">
         <v>33</v>
@@ -4896,7 +4897,7 @@
     </row>
     <row r="261" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A261" s="5" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="H261" t="s">
         <v>36</v>
@@ -4904,23 +4905,23 @@
     </row>
     <row r="262" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A262" s="5" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="H262" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="263" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A263" s="5" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="H263" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
     </row>
     <row r="264" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A264" s="5" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="B264">
         <v>1084</v>
@@ -4934,7 +4935,7 @@
     </row>
     <row r="265" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A265" s="5" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="H265" t="s">
         <v>39</v>
@@ -4942,7 +4943,7 @@
     </row>
     <row r="266" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A266" s="5" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="B266">
         <v>1084</v>
@@ -4956,7 +4957,7 @@
     </row>
     <row r="267" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A267" s="5" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="H267" t="s">
         <v>37</v>
@@ -4964,7 +4965,7 @@
     </row>
     <row r="268" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A268" s="5" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="B268">
         <v>1084</v>
@@ -4978,7 +4979,7 @@
     </row>
     <row r="269" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A269" s="5" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B269">
         <v>1084</v>
@@ -4992,7 +4993,7 @@
     </row>
     <row r="270" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A270" s="5" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="H270" t="s">
         <v>110</v>
@@ -5000,15 +5001,15 @@
     </row>
     <row r="271" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A271" s="5" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="H271" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
     </row>
     <row r="272" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A272" s="5" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="H272" t="s">
         <v>111</v>
@@ -5016,7 +5017,7 @@
     </row>
     <row r="273" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A273" s="5" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="B273" t="s">
         <v>5</v>
@@ -5030,7 +5031,7 @@
     </row>
     <row r="274" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A274" s="5" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B274">
         <v>1224</v>
@@ -5041,7 +5042,7 @@
     </row>
     <row r="275" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A275" s="5" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="H275" t="s">
         <v>40</v>
@@ -5049,7 +5050,7 @@
     </row>
     <row r="276" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A276" s="5" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="B276">
         <v>1219</v>
@@ -5063,7 +5064,7 @@
     </row>
     <row r="277" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A277" s="5" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="B277">
         <v>1219</v>
@@ -5075,12 +5076,12 @@
         <v>98</v>
       </c>
       <c r="H277" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
     </row>
     <row r="278" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A278" s="5" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="B278">
         <v>1219</v>
@@ -5092,12 +5093,12 @@
         <v>98</v>
       </c>
       <c r="H278" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
     </row>
     <row r="279" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A279" s="5" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="B279">
         <v>1219</v>
@@ -5108,7 +5109,7 @@
     </row>
     <row r="280" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A280" s="5" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B280">
         <v>1084</v>
@@ -5119,7 +5120,7 @@
     </row>
     <row r="281" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A281" s="5" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="B281">
         <v>1084</v>
@@ -5133,7 +5134,7 @@
     </row>
     <row r="282" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A282" s="5" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="B282">
         <v>1084</v>
@@ -5147,7 +5148,7 @@
     </row>
     <row r="283" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A283" s="5" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B283">
         <v>1084</v>
@@ -5155,7 +5156,7 @@
     </row>
     <row r="284" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A284" s="5" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="B284">
         <v>1084</v>
@@ -5169,7 +5170,7 @@
     </row>
     <row r="285" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A285" s="5" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="B285">
         <v>1084</v>
@@ -5183,7 +5184,7 @@
     </row>
     <row r="286" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A286" s="5" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="B286">
         <v>1084</v>
@@ -5197,7 +5198,7 @@
     </row>
     <row r="287" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A287" s="5" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="B287">
         <v>1084</v>
@@ -5211,7 +5212,7 @@
     </row>
     <row r="288" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A288" s="5" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="B288">
         <v>1084</v>
@@ -5225,7 +5226,7 @@
     </row>
     <row r="289" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A289" s="5" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="B289">
         <v>1084</v>
@@ -5239,7 +5240,7 @@
     </row>
     <row r="290" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A290" s="5" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="B290">
         <v>1084</v>
@@ -5253,7 +5254,7 @@
     </row>
     <row r="291" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A291" s="5" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="B291">
         <v>1084</v>
@@ -5267,7 +5268,7 @@
     </row>
     <row r="292" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A292" s="5" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="B292">
         <v>1084</v>
@@ -5281,7 +5282,7 @@
     </row>
     <row r="293" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A293" s="5" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B293">
         <v>1084</v>
@@ -5295,7 +5296,7 @@
     </row>
     <row r="294" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A294" s="5" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="B294">
         <v>1084</v>
@@ -5309,7 +5310,7 @@
     </row>
     <row r="295" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A295" s="5" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="B295">
         <v>1084</v>
@@ -5317,7 +5318,7 @@
     </row>
     <row r="296" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A296" s="5" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="B296">
         <v>1084</v>
@@ -5325,7 +5326,7 @@
     </row>
     <row r="297" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A297" s="5" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B297">
         <v>1084</v>
@@ -5339,29 +5340,29 @@
     </row>
     <row r="298" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A298" s="5" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="B298">
         <v>1084</v>
       </c>
       <c r="H298" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
     </row>
     <row r="299" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A299" s="5" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="B299">
         <v>1084</v>
       </c>
       <c r="H299" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
     </row>
     <row r="300" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A300" s="5" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="B300">
         <v>1084</v>
@@ -5375,7 +5376,7 @@
     </row>
     <row r="301" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A301" s="5" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="H301" t="s">
         <v>33</v>
@@ -5383,7 +5384,7 @@
     </row>
     <row r="302" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A302" s="5" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="B302">
         <v>1084</v>
@@ -5395,12 +5396,12 @@
         <v>6918</v>
       </c>
       <c r="H302" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
     </row>
     <row r="303" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A303" s="5" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="B303">
         <v>1084</v>
@@ -5414,7 +5415,7 @@
     </row>
     <row r="304" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A304" s="5" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="H304" t="s">
         <v>110</v>
@@ -5422,31 +5423,31 @@
     </row>
     <row r="305" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A305" s="5" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="H305" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
     </row>
     <row r="306" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A306" s="5" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="H306" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="307" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A307" s="5" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="H307" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
     </row>
     <row r="308" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A308" s="5" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="H308" t="s">
         <v>111</v>
@@ -5454,7 +5455,7 @@
     </row>
     <row r="309" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A309" s="5" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="B309">
         <v>1125</v>
@@ -5468,7 +5469,7 @@
     </row>
     <row r="310" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A310" s="5" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="B310">
         <v>1125</v>
@@ -5482,7 +5483,7 @@
     </row>
     <row r="311" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A311" s="5" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="B311">
         <v>1125</v>
@@ -5494,12 +5495,12 @@
         <v>30560</v>
       </c>
       <c r="H311" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
     </row>
     <row r="312" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A312" s="5" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="B312">
         <v>1125</v>
@@ -5513,7 +5514,7 @@
     </row>
     <row r="313" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A313" s="5" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="B313">
         <v>1125</v>
@@ -5527,7 +5528,7 @@
     </row>
     <row r="314" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A314" s="5" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="B314">
         <v>1125</v>
@@ -5541,7 +5542,7 @@
     </row>
     <row r="315" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A315" s="5" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="B315">
         <v>1125</v>
@@ -5555,7 +5556,7 @@
     </row>
     <row r="316" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A316" s="5" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="B316">
         <v>1125</v>
@@ -5569,7 +5570,7 @@
     </row>
     <row r="317" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A317" s="5" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="H317" t="s">
         <v>33</v>
@@ -5577,7 +5578,7 @@
     </row>
     <row r="318" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A318" s="5" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="H318" t="s">
         <v>33</v>
@@ -5585,7 +5586,7 @@
     </row>
     <row r="319" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A319" s="5" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="B319">
         <v>1125</v>
@@ -5596,7 +5597,7 @@
     </row>
     <row r="320" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A320" s="5" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="H320" t="s">
         <v>33</v>
@@ -5604,7 +5605,7 @@
     </row>
     <row r="321" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A321" s="5" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="B321">
         <v>1125</v>
@@ -5618,15 +5619,15 @@
     </row>
     <row r="322" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A322" s="5" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="H322" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
     </row>
     <row r="323" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A323" s="5" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="H323" t="s">
         <v>111</v>
@@ -5634,7 +5635,7 @@
     </row>
     <row r="324" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A324" s="5" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="B324">
         <v>1219</v>
@@ -5645,7 +5646,7 @@
     </row>
     <row r="325" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A325" s="5" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="H325" t="s">
         <v>101</v>
@@ -5653,7 +5654,7 @@
     </row>
     <row r="326" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A326" s="5" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="B326">
         <v>1219</v>
@@ -5664,7 +5665,7 @@
     </row>
     <row r="327" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A327" s="5" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="B327">
         <v>1219</v>
@@ -5678,15 +5679,15 @@
     </row>
     <row r="328" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A328" s="5" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="H328" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
     </row>
     <row r="329" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A329" s="5" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="H329" t="s">
         <v>110</v>
@@ -5694,15 +5695,15 @@
     </row>
     <row r="330" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A330" s="5" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="H330" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
     </row>
     <row r="331" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A331" s="5" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="H331" t="s">
         <v>110</v>
@@ -5710,7 +5711,7 @@
     </row>
     <row r="332" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A332" s="5" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="H332" t="s">
         <v>76</v>
@@ -5718,7 +5719,7 @@
     </row>
     <row r="333" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A333" s="5" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="B333">
         <v>1219</v>
@@ -5732,7 +5733,7 @@
     </row>
     <row r="334" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A334" s="5" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="B334">
         <v>1219</v>
@@ -5749,7 +5750,7 @@
     </row>
     <row r="335" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A335" s="5" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="B335">
         <v>1219</v>
@@ -5763,7 +5764,7 @@
     </row>
     <row r="336" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A336" s="5" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="B336">
         <v>1219</v>
@@ -5777,7 +5778,7 @@
     </row>
     <row r="337" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A337" s="5" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="B337">
         <v>1219</v>
@@ -5791,7 +5792,7 @@
     </row>
     <row r="338" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A338" s="5" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="H338" t="s">
         <v>110</v>
@@ -5799,74 +5800,68 @@
     </row>
     <row r="339" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A339" s="5" t="s">
-        <v>355</v>
+        <v>354</v>
+      </c>
+      <c r="B339">
+        <v>1219</v>
+      </c>
+      <c r="C339">
+        <v>17</v>
       </c>
     </row>
     <row r="340" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A340" s="5" t="s">
-        <v>445</v>
-      </c>
-      <c r="H340" t="s">
-        <v>425</v>
+        <v>591</v>
+      </c>
+      <c r="B340">
+        <v>1219</v>
+      </c>
+      <c r="C340">
+        <v>17</v>
       </c>
     </row>
     <row r="341" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A341" s="5" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="H341" t="s">
-        <v>111</v>
+        <v>424</v>
       </c>
     </row>
     <row r="342" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A342" s="5" t="s">
-        <v>356</v>
-      </c>
-      <c r="B342">
-        <v>1175</v>
-      </c>
-      <c r="C342">
-        <v>310</v>
-      </c>
-      <c r="D342">
-        <v>6941</v>
-      </c>
-      <c r="E342" t="s">
-        <v>23</v>
-      </c>
-      <c r="F342">
-        <v>410</v>
-      </c>
-      <c r="G342">
-        <v>6941</v>
+        <v>445</v>
+      </c>
+      <c r="H342" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="343" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A343" s="5" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="B343">
         <v>1175</v>
       </c>
       <c r="C343">
-        <v>320</v>
+        <v>310</v>
       </c>
       <c r="D343">
-        <v>6940</v>
+        <v>6941</v>
       </c>
       <c r="E343" t="s">
         <v>23</v>
       </c>
       <c r="F343">
-        <v>420</v>
+        <v>410</v>
       </c>
       <c r="G343">
-        <v>6940</v>
+        <v>6941</v>
       </c>
     </row>
     <row r="344" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A344" s="5" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="B344">
         <v>1175</v>
@@ -5875,7 +5870,7 @@
         <v>320</v>
       </c>
       <c r="D344">
-        <v>6939</v>
+        <v>6940</v>
       </c>
       <c r="E344" t="s">
         <v>23</v>
@@ -5884,12 +5879,12 @@
         <v>420</v>
       </c>
       <c r="G344">
-        <v>6939</v>
+        <v>6940</v>
       </c>
     </row>
     <row r="345" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A345" s="5" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="B345">
         <v>1175</v>
@@ -5898,7 +5893,7 @@
         <v>320</v>
       </c>
       <c r="D345">
-        <v>6944</v>
+        <v>6939</v>
       </c>
       <c r="E345" t="s">
         <v>23</v>
@@ -5907,12 +5902,12 @@
         <v>420</v>
       </c>
       <c r="G345">
-        <v>6944</v>
+        <v>6939</v>
       </c>
     </row>
     <row r="346" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A346" s="5" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="B346">
         <v>1175</v>
@@ -5921,7 +5916,7 @@
         <v>320</v>
       </c>
       <c r="D346">
-        <v>6943</v>
+        <v>6944</v>
       </c>
       <c r="E346" t="s">
         <v>23</v>
@@ -5930,12 +5925,12 @@
         <v>420</v>
       </c>
       <c r="G346">
-        <v>6943</v>
+        <v>6944</v>
       </c>
     </row>
     <row r="347" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A347" s="5" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="B347">
         <v>1175</v>
@@ -5944,7 +5939,7 @@
         <v>320</v>
       </c>
       <c r="D347">
-        <v>117</v>
+        <v>6943</v>
       </c>
       <c r="E347" t="s">
         <v>23</v>
@@ -5953,214 +5948,223 @@
         <v>420</v>
       </c>
       <c r="G347">
-        <v>117</v>
+        <v>6943</v>
       </c>
     </row>
     <row r="348" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A348" s="5" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="B348">
         <v>1175</v>
       </c>
       <c r="C348">
-        <v>330</v>
+        <v>320</v>
       </c>
       <c r="D348">
-        <v>27430</v>
-      </c>
-      <c r="E348">
-        <v>1167.1368</v>
+        <v>117</v>
+      </c>
+      <c r="E348" t="s">
+        <v>23</v>
       </c>
       <c r="F348">
-        <v>430</v>
+        <v>420</v>
       </c>
       <c r="G348">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="349" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A349" s="5" t="s">
-        <v>363</v>
-      </c>
-      <c r="E349" t="s">
-        <v>23</v>
+        <v>361</v>
+      </c>
+      <c r="B349">
+        <v>1175</v>
+      </c>
+      <c r="C349">
+        <v>330</v>
+      </c>
+      <c r="D349">
+        <v>27430</v>
+      </c>
+      <c r="E349">
+        <v>1167.1368</v>
       </c>
       <c r="F349">
-        <v>440</v>
+        <v>430</v>
       </c>
       <c r="G349">
-        <v>7128</v>
+        <v>118</v>
       </c>
     </row>
     <row r="350" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A350" s="5" t="s">
-        <v>364</v>
-      </c>
-      <c r="B350">
-        <v>1175</v>
-      </c>
-      <c r="C350">
-        <v>320</v>
-      </c>
-      <c r="D350">
-        <v>117</v>
+        <v>362</v>
       </c>
       <c r="E350" t="s">
         <v>23</v>
       </c>
       <c r="F350">
-        <v>420</v>
+        <v>440</v>
       </c>
       <c r="G350">
-        <v>117</v>
-      </c>
-      <c r="H350" t="s">
-        <v>91</v>
+        <v>7128</v>
       </c>
     </row>
     <row r="351" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A351" s="5" t="s">
-        <v>365</v>
+        <v>363</v>
+      </c>
+      <c r="B351">
+        <v>1175</v>
+      </c>
+      <c r="C351">
+        <v>320</v>
+      </c>
+      <c r="D351">
+        <v>117</v>
       </c>
       <c r="E351" t="s">
         <v>23</v>
       </c>
       <c r="F351">
-        <v>450</v>
+        <v>420</v>
       </c>
       <c r="G351">
-        <v>287</v>
+        <v>117</v>
+      </c>
+      <c r="H351" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="352" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A352" s="5" t="s">
-        <v>366</v>
-      </c>
-      <c r="H352" t="s">
-        <v>110</v>
+        <v>364</v>
+      </c>
+      <c r="E352" t="s">
+        <v>23</v>
+      </c>
+      <c r="F352">
+        <v>450</v>
+      </c>
+      <c r="G352">
+        <v>287</v>
       </c>
     </row>
     <row r="353" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A353" s="5" t="s">
-        <v>447</v>
+        <v>365</v>
       </c>
       <c r="H353" t="s">
-        <v>425</v>
+        <v>110</v>
       </c>
     </row>
     <row r="354" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A354" s="5" t="s">
-        <v>367</v>
+        <v>446</v>
       </c>
       <c r="H354" t="s">
-        <v>111</v>
+        <v>424</v>
       </c>
     </row>
     <row r="355" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A355" s="5" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="H355" t="s">
-        <v>92</v>
+        <v>111</v>
       </c>
     </row>
     <row r="356" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A356" s="5" t="s">
-        <v>369</v>
-      </c>
-      <c r="B356" t="s">
-        <v>24</v>
-      </c>
-      <c r="C356">
-        <v>110</v>
-      </c>
-      <c r="D356" t="s">
-        <v>47</v>
+        <v>367</v>
+      </c>
+      <c r="H356" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="357" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A357" s="5" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="B357" t="s">
         <v>24</v>
       </c>
       <c r="C357">
-        <v>120</v>
+        <v>110</v>
       </c>
       <c r="D357" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="358" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A358" s="5" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="B358" t="s">
         <v>24</v>
       </c>
       <c r="C358">
-        <v>130</v>
+        <v>120</v>
       </c>
       <c r="D358" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="359" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A359" s="5" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="B359" t="s">
         <v>24</v>
       </c>
       <c r="C359">
-        <v>140</v>
+        <v>130</v>
       </c>
       <c r="D359" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="360" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A360" s="5" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="B360" t="s">
         <v>24</v>
       </c>
       <c r="C360">
-        <v>150</v>
+        <v>140</v>
       </c>
       <c r="D360" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="361" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A361" s="5" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="B361" t="s">
         <v>24</v>
       </c>
       <c r="C361">
-        <v>160</v>
+        <v>150</v>
       </c>
       <c r="D361" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="362" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A362" s="5" t="s">
-        <v>424</v>
-      </c>
-      <c r="B362">
-        <v>1175</v>
+        <v>373</v>
+      </c>
+      <c r="B362" t="s">
+        <v>24</v>
       </c>
       <c r="C362">
-        <v>165</v>
-      </c>
-      <c r="D362">
-        <v>31625</v>
+        <v>160</v>
+      </c>
+      <c r="D362" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="363" spans="1:8" x14ac:dyDescent="0.3">
@@ -6168,50 +6172,56 @@
         <v>423</v>
       </c>
       <c r="B363">
-        <v>1175.1167</v>
+        <v>1175</v>
       </c>
       <c r="C363">
-        <v>170</v>
-      </c>
-      <c r="D363" t="s">
-        <v>53</v>
+        <v>165</v>
+      </c>
+      <c r="D363">
+        <v>31625</v>
       </c>
     </row>
     <row r="364" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A364" s="5" t="s">
         <v>422</v>
       </c>
-      <c r="H364" t="s">
-        <v>110</v>
+      <c r="B364">
+        <v>1175.1167</v>
+      </c>
+      <c r="C364">
+        <v>170</v>
+      </c>
+      <c r="D364" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="365" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A365" s="5" t="s">
-        <v>448</v>
+        <v>421</v>
       </c>
       <c r="H365" t="s">
-        <v>425</v>
+        <v>110</v>
       </c>
     </row>
     <row r="366" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A366" s="5" t="s">
-        <v>375</v>
+        <v>447</v>
       </c>
       <c r="H366" t="s">
-        <v>111</v>
+        <v>424</v>
       </c>
     </row>
     <row r="367" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A367" s="5" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="H367" t="s">
-        <v>33</v>
+        <v>111</v>
       </c>
     </row>
     <row r="368" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A368" s="5" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="H368" t="s">
         <v>33</v>
@@ -6219,7 +6229,7 @@
     </row>
     <row r="369" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A369" s="5" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="H369" t="s">
         <v>33</v>
@@ -6227,95 +6237,89 @@
     </row>
     <row r="370" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A370" s="5" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="H370" t="s">
-        <v>103</v>
+        <v>33</v>
       </c>
     </row>
     <row r="371" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A371" s="5" t="s">
-        <v>449</v>
+        <v>378</v>
       </c>
       <c r="H371" t="s">
-        <v>425</v>
+        <v>103</v>
       </c>
     </row>
     <row r="372" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A372" s="5" t="s">
-        <v>132</v>
+        <v>448</v>
       </c>
       <c r="H372" t="s">
-        <v>111</v>
+        <v>424</v>
       </c>
     </row>
     <row r="373" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A373" s="5" t="s">
-        <v>583</v>
-      </c>
-      <c r="B373" t="s">
-        <v>5</v>
-      </c>
-      <c r="C373" t="s">
-        <v>16</v>
-      </c>
-      <c r="D373">
-        <v>19890</v>
+        <v>132</v>
+      </c>
+      <c r="H373" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="374" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A374" s="5" t="s">
-        <v>133</v>
-      </c>
-      <c r="H374" t="s">
-        <v>185</v>
+        <v>582</v>
+      </c>
+      <c r="B374" t="s">
+        <v>5</v>
+      </c>
+      <c r="C374" t="s">
+        <v>16</v>
+      </c>
+      <c r="D374">
+        <v>19890</v>
       </c>
     </row>
     <row r="375" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A375" s="5" t="s">
-        <v>134</v>
-      </c>
-      <c r="B375" t="s">
-        <v>5</v>
-      </c>
-      <c r="C375" t="s">
-        <v>16</v>
-      </c>
-      <c r="D375">
-        <v>19811</v>
+        <v>133</v>
+      </c>
+      <c r="H375" t="s">
+        <v>184</v>
       </c>
     </row>
     <row r="376" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A376" s="5" t="s">
-        <v>171</v>
+        <v>134</v>
       </c>
       <c r="B376" t="s">
         <v>5</v>
       </c>
       <c r="C376" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D376">
-        <v>19791</v>
+        <v>19811</v>
       </c>
     </row>
     <row r="377" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A377" s="5" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B377" t="s">
         <v>5</v>
       </c>
       <c r="C377" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D377">
-        <v>19792</v>
+        <v>19791</v>
       </c>
     </row>
     <row r="378" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A378" s="5" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="B378" t="s">
         <v>5</v>
@@ -6329,43 +6333,43 @@
     </row>
     <row r="379" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A379" s="5" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="B379" t="s">
         <v>5</v>
       </c>
       <c r="C379" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D379">
-        <v>19794</v>
+        <v>19792</v>
       </c>
     </row>
     <row r="380" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A380" s="5" t="s">
-        <v>135</v>
-      </c>
-      <c r="H380" t="s">
-        <v>110</v>
+        <v>173</v>
+      </c>
+      <c r="B380" t="s">
+        <v>5</v>
+      </c>
+      <c r="C380" t="s">
+        <v>19</v>
+      </c>
+      <c r="D380">
+        <v>19794</v>
       </c>
     </row>
     <row r="381" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A381" s="5" t="s">
-        <v>136</v>
-      </c>
-      <c r="B381" t="s">
-        <v>5</v>
-      </c>
-      <c r="C381" t="s">
-        <v>93</v>
-      </c>
-      <c r="D381">
-        <v>19795</v>
+        <v>135</v>
+      </c>
+      <c r="H381" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="382" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A382" s="5" t="s">
-        <v>414</v>
+        <v>136</v>
       </c>
       <c r="B382" t="s">
         <v>5</v>
@@ -6379,152 +6383,151 @@
     </row>
     <row r="383" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A383" s="5" t="s">
-        <v>415</v>
-      </c>
-      <c r="H383" t="s">
-        <v>110</v>
+        <v>413</v>
+      </c>
+      <c r="B383" t="s">
+        <v>5</v>
+      </c>
+      <c r="C383" t="s">
+        <v>93</v>
+      </c>
+      <c r="D383">
+        <v>19795</v>
       </c>
     </row>
     <row r="384" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A384" s="5" t="s">
-        <v>450</v>
-      </c>
-      <c r="B384">
-        <v>1177</v>
-      </c>
-      <c r="C384">
-        <v>329</v>
-      </c>
-      <c r="D384">
-        <v>19723</v>
+        <v>414</v>
+      </c>
+      <c r="H384" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="385" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A385" s="5" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
       <c r="B385">
         <v>1177</v>
       </c>
       <c r="C385">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="D385">
-        <v>33016</v>
+        <v>19723</v>
       </c>
     </row>
     <row r="386" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A386" s="5" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
       <c r="B386">
         <v>1177</v>
       </c>
       <c r="C386">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="D386">
-        <v>12468</v>
+        <v>33016</v>
       </c>
     </row>
     <row r="387" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A387" s="5" t="s">
-        <v>453</v>
-      </c>
-      <c r="H387" t="s">
-        <v>110</v>
+        <v>451</v>
+      </c>
+      <c r="B387">
+        <v>1177</v>
+      </c>
+      <c r="C387">
+        <v>332</v>
+      </c>
+      <c r="D387">
+        <v>12468</v>
       </c>
     </row>
     <row r="388" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A388" s="5" t="s">
-        <v>454</v>
-      </c>
-      <c r="B388">
-        <v>1177</v>
-      </c>
-      <c r="C388">
-        <v>343</v>
-      </c>
-      <c r="D388">
-        <v>37299</v>
+        <v>452</v>
+      </c>
+      <c r="H388" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="389" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A389" s="5" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="B389">
         <v>1177</v>
       </c>
       <c r="C389">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="D389">
-        <v>37785</v>
+        <v>37299</v>
       </c>
     </row>
     <row r="390" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A390" s="5" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
       <c r="B390">
         <v>1177</v>
       </c>
       <c r="C390">
-        <v>347</v>
+        <v>344</v>
       </c>
       <c r="D390">
-        <v>12471</v>
+        <v>37785</v>
       </c>
     </row>
     <row r="391" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A391" s="5" t="s">
-        <v>457</v>
-      </c>
-      <c r="H391" t="s">
-        <v>110</v>
+        <v>455</v>
+      </c>
+      <c r="B391">
+        <v>1177</v>
+      </c>
+      <c r="C391">
+        <v>347</v>
+      </c>
+      <c r="D391">
+        <v>12471</v>
       </c>
     </row>
     <row r="392" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A392" s="5" t="s">
-        <v>458</v>
-      </c>
-      <c r="B392">
-        <v>1177</v>
-      </c>
-      <c r="C392">
-        <v>349</v>
-      </c>
-      <c r="D392">
-        <v>19774</v>
+        <v>456</v>
+      </c>
+      <c r="H392" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="393" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A393" s="5" t="s">
-        <v>459</v>
-      </c>
-      <c r="H393" t="s">
-        <v>110</v>
+        <v>457</v>
+      </c>
+      <c r="B393">
+        <v>1177</v>
+      </c>
+      <c r="C393">
+        <v>349</v>
+      </c>
+      <c r="D393">
+        <v>19774</v>
       </c>
     </row>
     <row r="394" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A394" s="5" t="s">
-        <v>460</v>
-      </c>
-      <c r="B394">
-        <v>1177</v>
-      </c>
-      <c r="C394">
-        <v>333</v>
-      </c>
-      <c r="D394">
-        <v>12472</v>
-      </c>
-      <c r="J394" s="1"/>
+        <v>458</v>
+      </c>
+      <c r="H394" t="s">
+        <v>110</v>
+      </c>
     </row>
     <row r="395" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A395" s="5" t="s">
-        <v>464</v>
+        <v>459</v>
       </c>
       <c r="B395">
         <v>1177</v>
@@ -6533,12 +6536,13 @@
         <v>333</v>
       </c>
       <c r="D395">
-        <v>12474</v>
-      </c>
+        <v>12472</v>
+      </c>
+      <c r="J395" s="1"/>
     </row>
     <row r="396" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A396" s="5" t="s">
-        <v>461</v>
+        <v>463</v>
       </c>
       <c r="B396">
         <v>1177</v>
@@ -6547,248 +6551,248 @@
         <v>333</v>
       </c>
       <c r="D396">
-        <v>19772</v>
+        <v>12474</v>
       </c>
     </row>
     <row r="397" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A397" s="5" t="s">
-        <v>462</v>
-      </c>
-      <c r="H397" t="s">
-        <v>425</v>
+        <v>460</v>
+      </c>
+      <c r="B397">
+        <v>1177</v>
+      </c>
+      <c r="C397">
+        <v>333</v>
+      </c>
+      <c r="D397">
+        <v>19772</v>
       </c>
     </row>
     <row r="398" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A398" s="5" t="s">
-        <v>145</v>
+        <v>461</v>
       </c>
       <c r="H398" t="s">
-        <v>111</v>
+        <v>424</v>
       </c>
     </row>
     <row r="399" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A399" s="5" t="s">
-        <v>584</v>
-      </c>
-      <c r="B399">
-        <v>1224</v>
-      </c>
-      <c r="D399">
-        <v>19812</v>
+        <v>145</v>
+      </c>
+      <c r="H399" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="400" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A400" s="5" t="s">
-        <v>175</v>
+        <v>583</v>
       </c>
       <c r="B400">
         <v>1224</v>
       </c>
-      <c r="C400" s="2" t="s">
-        <v>20</v>
-      </c>
       <c r="D400">
-        <v>26167</v>
+        <v>19812</v>
       </c>
     </row>
     <row r="401" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A401" s="5" t="s">
-        <v>585</v>
+        <v>174</v>
       </c>
       <c r="B401">
         <v>1224</v>
       </c>
-      <c r="C401" s="3" t="s">
-        <v>586</v>
+      <c r="C401" s="2" t="s">
+        <v>20</v>
       </c>
       <c r="D401">
-        <v>26168</v>
+        <v>26167</v>
       </c>
     </row>
     <row r="402" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A402" s="5" t="s">
-        <v>587</v>
+        <v>584</v>
       </c>
       <c r="B402">
         <v>1224</v>
       </c>
       <c r="C402" s="3" t="s">
-        <v>588</v>
+        <v>585</v>
       </c>
       <c r="D402">
-        <v>26169</v>
+        <v>26168</v>
       </c>
     </row>
     <row r="403" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A403" s="5" t="s">
-        <v>176</v>
+        <v>586</v>
       </c>
       <c r="B403">
         <v>1224</v>
       </c>
       <c r="C403" s="3" t="s">
-        <v>21</v>
+        <v>587</v>
       </c>
       <c r="D403">
-        <v>26733</v>
+        <v>26169</v>
       </c>
     </row>
     <row r="404" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A404" s="5" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="B404">
         <v>1224</v>
       </c>
       <c r="C404" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="D404" s="3">
-        <v>30788</v>
+        <v>21</v>
+      </c>
+      <c r="D404">
+        <v>26733</v>
       </c>
     </row>
     <row r="405" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A405" s="5" t="s">
-        <v>137</v>
-      </c>
-      <c r="C405" s="2"/>
-      <c r="D405" s="3"/>
-      <c r="H405" t="s">
-        <v>110</v>
+        <v>176</v>
+      </c>
+      <c r="B405">
+        <v>1224</v>
+      </c>
+      <c r="C405" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D405" s="3">
+        <v>30788</v>
       </c>
     </row>
     <row r="406" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A406" s="5" t="s">
-        <v>178</v>
-      </c>
-      <c r="B406">
-        <v>1224</v>
-      </c>
-      <c r="C406" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="D406" s="3">
-        <v>2028</v>
+        <v>137</v>
+      </c>
+      <c r="C406" s="2"/>
+      <c r="D406" s="3"/>
+      <c r="H406" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="407" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A407" s="5" t="s">
-        <v>138</v>
-      </c>
-      <c r="C407" s="2"/>
-      <c r="D407" s="3"/>
-      <c r="H407" t="s">
-        <v>110</v>
+        <v>177</v>
+      </c>
+      <c r="B407">
+        <v>1224</v>
+      </c>
+      <c r="C407" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="D407" s="3">
+        <v>2028</v>
       </c>
     </row>
     <row r="408" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A408" s="5" t="s">
-        <v>179</v>
-      </c>
-      <c r="B408">
-        <v>1224</v>
-      </c>
-      <c r="C408" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="D408" s="3">
-        <v>26144</v>
+        <v>138</v>
+      </c>
+      <c r="C408" s="2"/>
+      <c r="D408" s="3"/>
+      <c r="H408" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="409" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A409" s="5" t="s">
-        <v>139</v>
-      </c>
-      <c r="C409" s="2"/>
-      <c r="D409" s="3"/>
-      <c r="H409" t="s">
-        <v>110</v>
+        <v>178</v>
+      </c>
+      <c r="B409">
+        <v>1224</v>
+      </c>
+      <c r="C409" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="D409" s="3">
+        <v>26144</v>
       </c>
     </row>
     <row r="410" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A410" s="5" t="s">
-        <v>180</v>
-      </c>
-      <c r="B410">
-        <v>1224</v>
-      </c>
-      <c r="C410" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="D410" s="3">
-        <v>26172</v>
+        <v>139</v>
+      </c>
+      <c r="C410" s="2"/>
+      <c r="D410" s="3"/>
+      <c r="H410" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="411" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A411" s="5" t="s">
-        <v>140</v>
-      </c>
-      <c r="C411" s="2"/>
-      <c r="D411" s="3"/>
-      <c r="H411" t="s">
-        <v>110</v>
+        <v>179</v>
+      </c>
+      <c r="B411">
+        <v>1224</v>
+      </c>
+      <c r="C411" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="D411" s="3">
+        <v>26172</v>
       </c>
     </row>
     <row r="412" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A412" s="5" t="s">
-        <v>141</v>
-      </c>
-      <c r="B412">
-        <v>1224</v>
-      </c>
-      <c r="C412" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="D412" s="3">
-        <v>26171</v>
+        <v>140</v>
+      </c>
+      <c r="C412" s="2"/>
+      <c r="D412" s="3"/>
+      <c r="H412" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="413" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A413" s="5" t="s">
-        <v>463</v>
-      </c>
-      <c r="H413" t="s">
-        <v>425</v>
+        <v>141</v>
+      </c>
+      <c r="B413">
+        <v>1224</v>
+      </c>
+      <c r="C413" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D413" s="3">
+        <v>26171</v>
       </c>
     </row>
     <row r="414" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A414" s="5" t="s">
-        <v>143</v>
-      </c>
-      <c r="C414" s="4"/>
+        <v>462</v>
+      </c>
       <c r="H414" t="s">
-        <v>111</v>
+        <v>424</v>
       </c>
     </row>
     <row r="415" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A415" s="5" t="s">
-        <v>144</v>
-      </c>
-      <c r="B415">
-        <v>1224</v>
+        <v>143</v>
       </c>
       <c r="C415" s="4"/>
       <c r="H415" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
     </row>
     <row r="416" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A416" s="5" t="s">
-        <v>182</v>
+        <v>144</v>
       </c>
       <c r="B416">
         <v>1224</v>
       </c>
-      <c r="C416" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="D416" t="s">
-        <v>107</v>
+      <c r="C416" s="4"/>
+      <c r="H416" t="s">
+        <v>109</v>
       </c>
     </row>
     <row r="417" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A417" s="5" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="B417">
         <v>1224</v>
@@ -6797,166 +6801,180 @@
         <v>106</v>
       </c>
       <c r="D417" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="418" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A418" s="5" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="B418">
         <v>1224</v>
       </c>
       <c r="C418" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="D418" s="3">
-        <v>26173</v>
+        <v>106</v>
+      </c>
+      <c r="D418" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="419" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A419" s="5" t="s">
-        <v>142</v>
-      </c>
-      <c r="C419" s="2"/>
-      <c r="D419" s="3"/>
-      <c r="H419" t="s">
-        <v>110</v>
+        <v>180</v>
+      </c>
+      <c r="B419">
+        <v>1224</v>
+      </c>
+      <c r="C419" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D419" s="3">
+        <v>26173</v>
       </c>
     </row>
     <row r="420" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A420" s="5" t="s">
-        <v>146</v>
-      </c>
+        <v>142</v>
+      </c>
+      <c r="C420" s="2"/>
+      <c r="D420" s="3"/>
       <c r="H420" t="s">
-        <v>99</v>
+        <v>110</v>
       </c>
     </row>
     <row r="421" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A421" s="5" t="s">
-        <v>147</v>
+        <v>590</v>
       </c>
       <c r="H421" t="s">
-        <v>112</v>
+        <v>589</v>
       </c>
     </row>
     <row r="422" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A422" s="5" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="H422" t="s">
-        <v>590</v>
+        <v>99</v>
       </c>
     </row>
     <row r="423" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A423" s="5" t="s">
-        <v>545</v>
+        <v>147</v>
       </c>
       <c r="H423" t="s">
-        <v>425</v>
+        <v>112</v>
       </c>
     </row>
     <row r="424" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A424" s="5" t="s">
-        <v>546</v>
+        <v>544</v>
       </c>
       <c r="H424" t="s">
-        <v>111</v>
+        <v>424</v>
       </c>
     </row>
     <row r="425" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A425" s="5" t="s">
-        <v>547</v>
+        <v>545</v>
       </c>
       <c r="H425" t="s">
-        <v>33</v>
+        <v>111</v>
       </c>
     </row>
     <row r="426" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A426" s="5" t="s">
-        <v>548</v>
+        <v>546</v>
       </c>
       <c r="H426" t="s">
-        <v>110</v>
+        <v>33</v>
       </c>
     </row>
     <row r="427" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A427" s="5" t="s">
-        <v>549</v>
+        <v>547</v>
       </c>
       <c r="H427" t="s">
-        <v>33</v>
+        <v>110</v>
       </c>
     </row>
     <row r="428" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A428" s="5" t="s">
-        <v>550</v>
+        <v>548</v>
       </c>
       <c r="H428" t="s">
-        <v>110</v>
+        <v>33</v>
       </c>
     </row>
     <row r="429" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A429" s="5" t="s">
-        <v>551</v>
+        <v>549</v>
       </c>
       <c r="H429" t="s">
-        <v>33</v>
+        <v>110</v>
       </c>
     </row>
     <row r="430" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A430" s="5" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
       <c r="H430" t="s">
-        <v>110</v>
+        <v>33</v>
       </c>
     </row>
     <row r="431" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A431" s="5" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
       <c r="H431" t="s">
-        <v>33</v>
+        <v>110</v>
       </c>
     </row>
     <row r="432" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A432" s="5" t="s">
-        <v>554</v>
+        <v>552</v>
       </c>
       <c r="H432" t="s">
-        <v>110</v>
+        <v>33</v>
       </c>
     </row>
     <row r="433" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A433" s="5" t="s">
-        <v>555</v>
+        <v>553</v>
       </c>
       <c r="H433" t="s">
-        <v>33</v>
+        <v>110</v>
       </c>
     </row>
     <row r="434" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A434" s="5" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="H434" t="s">
-        <v>110</v>
+        <v>33</v>
       </c>
     </row>
     <row r="435" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A435" s="5" t="s">
-        <v>557</v>
+        <v>555</v>
       </c>
       <c r="H435" t="s">
-        <v>33</v>
+        <v>110</v>
       </c>
     </row>
     <row r="436" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A436" s="5" t="s">
-        <v>558</v>
+        <v>556</v>
       </c>
       <c r="H436" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="437" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A437" s="5" t="s">
+        <v>557</v>
+      </c>
+      <c r="H437" t="s">
         <v>110</v>
       </c>
     </row>

</xml_diff>